<commit_message>
Expanded to allow for off the money pricing example
</commit_message>
<xml_diff>
--- a/BBG/Volcubes.xlsx
+++ b/BBG/Volcubes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Desktop\Other\SwaptionPricing\BBG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Desktop\Other\Black76\BBG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3FD957-AE7B-4124-B964-61ED62017990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C5A9A4-E333-4584-BCBF-6AE6878EE188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,7 @@
     <sheet name="black_vols" sheetId="1" r:id="rId1"/>
     <sheet name="black_strikes" sheetId="5" r:id="rId2"/>
     <sheet name="normal_vols" sheetId="2" r:id="rId3"/>
-    <sheet name="normal225" sheetId="3" r:id="rId4"/>
-    <sheet name="quickpricer" sheetId="4" r:id="rId5"/>
+    <sheet name="black220_vols" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
-  <si>
-    <t>some assumptions for model:  continuous compounding, day count conventions are ignored, SONIA replaces LIBOR</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
   <si>
     <t>Expiry</t>
   </si>
@@ -281,23 +277,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>391428</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>48132</xdr:rowOff>
+      <xdr:colOff>257780</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95874</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43452558-0766-B976-5EAD-52A7344F2AEE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D749E6EB-306F-5B15-5126-ED60DDAE2154}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -313,8 +309,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6724650" y="2514600"/>
-          <a:ext cx="6468378" cy="3629532"/>
+          <a:off x="8724900" y="200025"/>
+          <a:ext cx="4334480" cy="4467849"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -592,14 +588,14 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -1310,14 +1306,14 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -2028,7 +2024,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,36 +2035,719 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5161B7-3F14-4C4F-A9D2-4E94C6FACD61}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FD7154-7717-4CE4-AAFB-AC944F49550F}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515F138A-F11D-4C5C-98F7-0BE8C2F51F2A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <f>1/12</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="B2">
+        <v>57.26</v>
+      </c>
+      <c r="C2">
+        <v>54.21</v>
+      </c>
+      <c r="D2">
+        <v>55.28</v>
+      </c>
+      <c r="E2">
+        <v>57.54</v>
+      </c>
+      <c r="F2">
+        <v>59.01</v>
+      </c>
+      <c r="G2">
+        <v>59.48</v>
+      </c>
+      <c r="H2">
+        <v>59.62</v>
+      </c>
+      <c r="I2">
+        <v>58.72</v>
+      </c>
+      <c r="J2">
+        <v>58.73</v>
+      </c>
+      <c r="K2">
+        <v>58.25</v>
+      </c>
+      <c r="L2">
+        <v>58.27</v>
+      </c>
+      <c r="M2">
+        <v>58.47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+      <c r="B3">
+        <v>55.77</v>
+      </c>
+      <c r="C3">
+        <v>49.47</v>
+      </c>
+      <c r="D3">
+        <v>51.2</v>
+      </c>
+      <c r="E3">
+        <v>53.38</v>
+      </c>
+      <c r="F3">
+        <v>55.18</v>
+      </c>
+      <c r="G3">
+        <v>55.18</v>
+      </c>
+      <c r="H3">
+        <v>54.12</v>
+      </c>
+      <c r="I3">
+        <v>54.19</v>
+      </c>
+      <c r="J3">
+        <v>54.37</v>
+      </c>
+      <c r="K3">
+        <v>53.81</v>
+      </c>
+      <c r="L3">
+        <v>54.07</v>
+      </c>
+      <c r="M3">
+        <v>54.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f>6/12</f>
+        <v>0.5</v>
+      </c>
+      <c r="B4">
+        <v>57.1</v>
+      </c>
+      <c r="C4">
+        <v>50.43</v>
+      </c>
+      <c r="D4">
+        <v>50.55</v>
+      </c>
+      <c r="E4">
+        <v>51.37</v>
+      </c>
+      <c r="F4">
+        <v>51.87</v>
+      </c>
+      <c r="G4">
+        <v>51.85</v>
+      </c>
+      <c r="H4">
+        <v>50.63</v>
+      </c>
+      <c r="I4">
+        <v>50.69</v>
+      </c>
+      <c r="J4">
+        <v>50.82</v>
+      </c>
+      <c r="K4">
+        <v>50.26</v>
+      </c>
+      <c r="L4">
+        <v>50.29</v>
+      </c>
+      <c r="M4">
+        <v>50.24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <f>9/12</f>
+        <v>0.75</v>
+      </c>
+      <c r="B5">
+        <v>55.48</v>
+      </c>
+      <c r="C5">
+        <v>50.54</v>
+      </c>
+      <c r="D5">
+        <v>50.86</v>
+      </c>
+      <c r="E5">
+        <v>51.2</v>
+      </c>
+      <c r="F5">
+        <v>50.94</v>
+      </c>
+      <c r="G5">
+        <v>50.84</v>
+      </c>
+      <c r="H5">
+        <v>49.01</v>
+      </c>
+      <c r="I5">
+        <v>49.06</v>
+      </c>
+      <c r="J5">
+        <v>49.15</v>
+      </c>
+      <c r="K5">
+        <v>48.71</v>
+      </c>
+      <c r="L5">
+        <v>48.44</v>
+      </c>
+      <c r="M5">
+        <v>48.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>52.75</v>
+      </c>
+      <c r="C6">
+        <v>50.47</v>
+      </c>
+      <c r="D6">
+        <v>50.44</v>
+      </c>
+      <c r="E6">
+        <v>50.26</v>
+      </c>
+      <c r="F6">
+        <v>49.55</v>
+      </c>
+      <c r="G6">
+        <v>49.3</v>
+      </c>
+      <c r="H6">
+        <v>46.97</v>
+      </c>
+      <c r="I6">
+        <v>47.06</v>
+      </c>
+      <c r="J6">
+        <v>47.16</v>
+      </c>
+      <c r="K6">
+        <v>46.73</v>
+      </c>
+      <c r="L6">
+        <v>46.63</v>
+      </c>
+      <c r="M6">
+        <v>46.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>53.12</v>
+      </c>
+      <c r="C7">
+        <v>52.76</v>
+      </c>
+      <c r="D7">
+        <v>52.27</v>
+      </c>
+      <c r="E7">
+        <v>51.26</v>
+      </c>
+      <c r="F7">
+        <v>49.26</v>
+      </c>
+      <c r="G7">
+        <v>47.73</v>
+      </c>
+      <c r="H7">
+        <v>44.89</v>
+      </c>
+      <c r="I7">
+        <v>44.85</v>
+      </c>
+      <c r="J7">
+        <v>44.44</v>
+      </c>
+      <c r="K7">
+        <v>43.97</v>
+      </c>
+      <c r="L7">
+        <v>43.45</v>
+      </c>
+      <c r="M7">
+        <v>43.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>53.4</v>
+      </c>
+      <c r="C8">
+        <v>52.85</v>
+      </c>
+      <c r="D8">
+        <v>51.56</v>
+      </c>
+      <c r="E8">
+        <v>49.99</v>
+      </c>
+      <c r="F8">
+        <v>48.35</v>
+      </c>
+      <c r="G8">
+        <v>45.91</v>
+      </c>
+      <c r="H8">
+        <v>42.54</v>
+      </c>
+      <c r="I8">
+        <v>42.47</v>
+      </c>
+      <c r="J8">
+        <v>41.89</v>
+      </c>
+      <c r="K8">
+        <v>41.18</v>
+      </c>
+      <c r="L8">
+        <v>40.630000000000003</v>
+      </c>
+      <c r="M8">
+        <v>40.14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>51.37</v>
+      </c>
+      <c r="C9">
+        <v>51.38</v>
+      </c>
+      <c r="D9">
+        <v>50.05</v>
+      </c>
+      <c r="E9">
+        <v>48.17</v>
+      </c>
+      <c r="F9">
+        <v>45.92</v>
+      </c>
+      <c r="G9">
+        <v>43.52</v>
+      </c>
+      <c r="H9">
+        <v>40.36</v>
+      </c>
+      <c r="I9">
+        <v>40.090000000000003</v>
+      </c>
+      <c r="J9">
+        <v>39.659999999999997</v>
+      </c>
+      <c r="K9">
+        <v>39.14</v>
+      </c>
+      <c r="L9">
+        <v>38.61</v>
+      </c>
+      <c r="M9">
+        <v>37.93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>49.75</v>
+      </c>
+      <c r="C10">
+        <v>48.89</v>
+      </c>
+      <c r="D10">
+        <v>47.21</v>
+      </c>
+      <c r="E10">
+        <v>45.29</v>
+      </c>
+      <c r="F10">
+        <v>43.36</v>
+      </c>
+      <c r="G10">
+        <v>41.11</v>
+      </c>
+      <c r="H10">
+        <v>38.67</v>
+      </c>
+      <c r="I10">
+        <v>38.35</v>
+      </c>
+      <c r="J10">
+        <v>37.81</v>
+      </c>
+      <c r="K10">
+        <v>37.15</v>
+      </c>
+      <c r="L10">
+        <v>36.409999999999997</v>
+      </c>
+      <c r="M10">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>47.7</v>
+      </c>
+      <c r="C11">
+        <v>46.81</v>
+      </c>
+      <c r="D11">
+        <v>45.09</v>
+      </c>
+      <c r="E11">
+        <v>43.35</v>
+      </c>
+      <c r="F11">
+        <v>41.64</v>
+      </c>
+      <c r="G11">
+        <v>39.770000000000003</v>
+      </c>
+      <c r="H11">
+        <v>37.450000000000003</v>
+      </c>
+      <c r="I11">
+        <v>36.979999999999997</v>
+      </c>
+      <c r="J11">
+        <v>36.28</v>
+      </c>
+      <c r="K11">
+        <v>35.33</v>
+      </c>
+      <c r="L11">
+        <v>34.409999999999997</v>
+      </c>
+      <c r="M11">
+        <v>33.770000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>45.24</v>
+      </c>
+      <c r="C12">
+        <v>43.96</v>
+      </c>
+      <c r="D12">
+        <v>42.54</v>
+      </c>
+      <c r="E12">
+        <v>41.21</v>
+      </c>
+      <c r="F12">
+        <v>39.9</v>
+      </c>
+      <c r="G12">
+        <v>38.450000000000003</v>
+      </c>
+      <c r="H12">
+        <v>36.32</v>
+      </c>
+      <c r="I12">
+        <v>35.869999999999997</v>
+      </c>
+      <c r="J12">
+        <v>35.270000000000003</v>
+      </c>
+      <c r="K12">
+        <v>34.380000000000003</v>
+      </c>
+      <c r="L12">
+        <v>33.479999999999997</v>
+      </c>
+      <c r="M12">
+        <v>32.86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>42.42</v>
+      </c>
+      <c r="C13">
+        <v>41.97</v>
+      </c>
+      <c r="D13">
+        <v>40.840000000000003</v>
+      </c>
+      <c r="E13">
+        <v>39.619999999999997</v>
+      </c>
+      <c r="F13">
+        <v>38.86</v>
+      </c>
+      <c r="G13">
+        <v>37.53</v>
+      </c>
+      <c r="H13">
+        <v>35.6</v>
+      </c>
+      <c r="I13">
+        <v>35.01</v>
+      </c>
+      <c r="J13">
+        <v>34.270000000000003</v>
+      </c>
+      <c r="K13">
+        <v>33.520000000000003</v>
+      </c>
+      <c r="L13">
+        <v>31.86</v>
+      </c>
+      <c r="M13">
+        <v>30.89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>40.72</v>
+      </c>
+      <c r="C14">
+        <v>40.380000000000003</v>
+      </c>
+      <c r="D14">
+        <v>39.46</v>
+      </c>
+      <c r="E14">
+        <v>38.729999999999997</v>
+      </c>
+      <c r="F14">
+        <v>37.840000000000003</v>
+      </c>
+      <c r="G14">
+        <v>36.93</v>
+      </c>
+      <c r="H14">
+        <v>35.119999999999997</v>
+      </c>
+      <c r="I14">
+        <v>34.549999999999997</v>
+      </c>
+      <c r="J14">
+        <v>33.99</v>
+      </c>
+      <c r="K14">
+        <v>32.840000000000003</v>
+      </c>
+      <c r="L14">
+        <v>31.11</v>
+      </c>
+      <c r="M14">
+        <v>30.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>39.25</v>
+      </c>
+      <c r="C15">
+        <v>38.65</v>
+      </c>
+      <c r="D15">
+        <v>38.33</v>
+      </c>
+      <c r="E15">
+        <v>37.78</v>
+      </c>
+      <c r="F15">
+        <v>37.119999999999997</v>
+      </c>
+      <c r="G15">
+        <v>36.25</v>
+      </c>
+      <c r="H15">
+        <v>34.78</v>
+      </c>
+      <c r="I15">
+        <v>34.31</v>
+      </c>
+      <c r="J15">
+        <v>33.47</v>
+      </c>
+      <c r="K15">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="L15">
+        <v>31.11</v>
+      </c>
+      <c r="M15">
+        <v>30.11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>40.19</v>
+      </c>
+      <c r="C16">
+        <v>38.64</v>
+      </c>
+      <c r="D16">
+        <v>37.74</v>
+      </c>
+      <c r="E16">
+        <v>37.25</v>
+      </c>
+      <c r="F16">
+        <v>36.82</v>
+      </c>
+      <c r="G16">
+        <v>35.869999999999997</v>
+      </c>
+      <c r="H16">
+        <v>34.630000000000003</v>
+      </c>
+      <c r="I16">
+        <v>34.03</v>
+      </c>
+      <c r="J16">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="K16">
+        <v>31.75</v>
+      </c>
+      <c r="L16">
+        <v>30.63</v>
+      </c>
+      <c r="M16">
+        <v>29.71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>40.17</v>
+      </c>
+      <c r="C17">
+        <v>37.119999999999997</v>
+      </c>
+      <c r="D17">
+        <v>36.729999999999997</v>
+      </c>
+      <c r="E17">
+        <v>35.93</v>
+      </c>
+      <c r="F17">
+        <v>35.229999999999997</v>
+      </c>
+      <c r="G17">
+        <v>34.81</v>
+      </c>
+      <c r="H17">
+        <v>34.090000000000003</v>
+      </c>
+      <c r="I17">
+        <v>33.42</v>
+      </c>
+      <c r="J17">
+        <v>32.33</v>
+      </c>
+      <c r="K17">
+        <v>30.57</v>
+      </c>
+      <c r="L17">
+        <v>28.82</v>
+      </c>
+      <c r="M17">
+        <v>27.76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>